<commit_message>
Updated Right-Only achievement to start with small Peach
</commit_message>
<xml_diff>
--- a/My Sets/_Hack_ Present Panic - A Princess Adventure (NES)/~Hack~ Present Panic - A Princess Adventure (NES) - Plans.xlsx
+++ b/My Sets/_Hack_ Present Panic - A Princess Adventure (NES)/~Hack~ Present Panic - A Princess Adventure (NES) - Plans.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="635" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="635"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Game Dec" sheetId="16" state="hidden" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Achievements!$B$1:$G$177</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Achievements!$B$1:$G$179</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Checklist!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Extras!$A$1:$F$57</definedName>
   </definedNames>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="137">
   <si>
     <t>Description</t>
   </si>
@@ -268,9 +268,6 @@
     <t>Early Present VI</t>
   </si>
   <si>
-    <t>Beat the game in under 7:00 minutes</t>
-  </si>
-  <si>
     <t>Candy Striper</t>
   </si>
   <si>
@@ -419,6 +416,45 @@
   </si>
   <si>
     <t>Power Up || Game Over</t>
+  </si>
+  <si>
+    <t>Beat level 2 in 15s or less</t>
+  </si>
+  <si>
+    <t>Fast Flight</t>
+  </si>
+  <si>
+    <t>Barbeque Bowser</t>
+  </si>
+  <si>
+    <t>Beat the game with fire flower power</t>
+  </si>
+  <si>
+    <t>Beat the game with candy cane power</t>
+  </si>
+  <si>
+    <t>Beat level 4 with blooper power</t>
+  </si>
+  <si>
+    <t>Frozen Calamari</t>
+  </si>
+  <si>
+    <t>Beat the game in under 6:00 minutes</t>
+  </si>
+  <si>
+    <t>Righteous Royalty</t>
+  </si>
+  <si>
+    <t>Become invulnerable to fireballs while wearing the candy cane suit</t>
+  </si>
+  <si>
+    <t>Flameproof Princess of Mirth</t>
+  </si>
+  <si>
+    <t>Sweet Victory</t>
+  </si>
+  <si>
+    <t>Beat level 1 without pressing the left start as small Peach</t>
   </si>
 </sst>
 </file>
@@ -780,10 +816,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G180"/>
+  <dimension ref="A1:G182"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,184 +858,175 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="5">
         <f>VLOOKUP(D2,Stats!$A$1:$B$10,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <f>VLOOKUP(D3,Stats!$A$1:$B$10,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <f>VLOOKUP(D4,Stats!$A$1:$B$10,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+    </row>
+    <row r="5" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <f>VLOOKUP(D5,Stats!$A$1:$B$10,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="F5" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <f>VLOOKUP(D6,Stats!$A$1:$B$10,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="F6" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="7">
-        <f>VLOOKUP(D7,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+        <v>15</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="7">
+        <v>17</v>
+      </c>
+      <c r="E8" s="5">
         <f>VLOOKUP(D8,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <f>VLOOKUP(D9,Stats!$A$1:$B$10,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="F9" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -1009,19 +1036,18 @@
         <v>84</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="7">
+        <v>9</v>
+      </c>
+      <c r="E10" s="5">
         <f>VLOOKUP(D10,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1031,63 +1057,60 @@
         <v>83</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="7">
+        <v>17</v>
+      </c>
+      <c r="E11" s="5">
         <f>VLOOKUP(D11,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="7">
+        <v>9</v>
+      </c>
+      <c r="E12" s="5">
         <f>VLOOKUP(D12,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="7">
+        <v>10</v>
+      </c>
+      <c r="E13" s="5">
         <f>VLOOKUP(D13,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+        <v>3</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1097,457 +1120,533 @@
         <v>81</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="5">
+        <f>VLOOKUP(D14,Stats!$A$1:$B$10,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="7">
-        <f>VLOOKUP(D14,Stats!$A$1:$B$10,2,FALSE)</f>
+      <c r="E15" s="5">
+        <f>VLOOKUP(D15,Stats!$A$1:$B$10,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>14</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="7">
-        <f>VLOOKUP(D15,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+    </row>
+    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>57</v>
+        <v>132</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="7">
+        <v>12</v>
+      </c>
+      <c r="E16" s="5">
         <f>VLOOKUP(D16,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+        <v>5</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <f>VLOOKUP(D17,Stats!$A$1:$B$10,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="F17" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>59</v>
+        <v>130</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="7">
+        <v>14</v>
+      </c>
+      <c r="E18" s="5">
         <f>VLOOKUP(D18,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+        <v>25</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>60</v>
+        <v>126</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="7">
+        <v>13</v>
+      </c>
+      <c r="E19" s="5">
         <f>VLOOKUP(D19,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+        <v>10</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>61</v>
+        <v>135</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="5">
         <f>VLOOKUP(D20,Stats!$A$1:$B$10,2,FALSE)</f>
         <v>10</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="F20" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="7">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5">
         <f>VLOOKUP(D21,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>25</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="7">
+        <v>17</v>
+      </c>
+      <c r="E22" s="5">
         <f>VLOOKUP(D22,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>25</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+        <v>2</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="5">
         <f>VLOOKUP(D23,Stats!$A$1:$B$10,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="F23" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="7">
+        <v>11</v>
+      </c>
+      <c r="E24" s="5">
         <f>VLOOKUP(D24,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+        <v>4</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="7">
+        <v>10</v>
+      </c>
+      <c r="E25" s="5">
         <f>VLOOKUP(D25,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+        <v>3</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="7">
+        <v>12</v>
+      </c>
+      <c r="E26" s="5">
         <f>VLOOKUP(D26,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+        <v>5</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="7">
+        <v>13</v>
+      </c>
+      <c r="E27" s="5">
         <f>VLOOKUP(D27,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+        <v>10</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="7">
+        <v>14</v>
+      </c>
+      <c r="E28" s="5">
         <f>VLOOKUP(D28,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+        <v>25</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="5">
         <f>VLOOKUP(D29,Stats!$A$1:$B$10,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="5">
+        <f>VLOOKUP(D30,Stats!$A$1:$B$10,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="5">
+        <f>VLOOKUP(D31,Stats!$A$1:$B$10,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="5">
+        <f>VLOOKUP(D32,Stats!$A$1:$B$10,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="5">
+        <f>VLOOKUP(D33,Stats!$A$1:$B$10,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="5">
+        <f>VLOOKUP(D34,Stats!$A$1:$B$10,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="5">
+        <f>VLOOKUP(D35,Stats!$A$1:$B$10,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="8"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="8"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="8"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="8"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="8"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -1615,13 +1714,13 @@
     </row>
     <row r="59" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="8"/>
-      <c r="C59" s="10"/>
+      <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="G59" s="5"/>
     </row>
     <row r="60" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
-      <c r="C60" s="10"/>
+      <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="G60" s="5"/>
     </row>
@@ -1651,13 +1750,13 @@
     </row>
     <row r="65" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="8"/>
-      <c r="C65" s="5"/>
+      <c r="C65" s="10"/>
       <c r="D65" s="5"/>
       <c r="G65" s="5"/>
     </row>
     <row r="66" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="8"/>
-      <c r="C66" s="5"/>
+      <c r="C66" s="10"/>
       <c r="D66" s="5"/>
       <c r="G66" s="5"/>
     </row>
@@ -1741,13 +1840,13 @@
     </row>
     <row r="80" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="8"/>
-      <c r="C80" s="10"/>
+      <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="G80" s="5"/>
     </row>
     <row r="81" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="8"/>
-      <c r="C81" s="10"/>
+      <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="G81" s="5"/>
     </row>
@@ -1787,12 +1886,11 @@
       <c r="D87" s="5"/>
       <c r="G87" s="5"/>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="8"/>
       <c r="C88" s="10"/>
       <c r="D88" s="5"/>
-      <c r="E88" s="7"/>
-      <c r="F88" s="7"/>
+      <c r="G88" s="5"/>
     </row>
     <row r="89" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="8"/>
@@ -1800,11 +1898,12 @@
       <c r="D89" s="5"/>
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="8"/>
       <c r="C90" s="10"/>
       <c r="D90" s="5"/>
-      <c r="G90" s="5"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="7"/>
     </row>
     <row r="91" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="8"/>
@@ -1816,23 +1915,22 @@
       <c r="B92" s="8"/>
       <c r="C92" s="10"/>
       <c r="D92" s="5"/>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G92" s="5"/>
+    </row>
+    <row r="93" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="8"/>
       <c r="C93" s="10"/>
       <c r="D93" s="5"/>
-      <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G93" s="5"/>
+    </row>
+    <row r="94" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="8"/>
       <c r="C94" s="10"/>
       <c r="D94" s="5"/>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="8"/>
+      <c r="C95" s="10"/>
       <c r="D95" s="5"/>
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
@@ -1845,9 +1943,16 @@
       <c r="F96" s="7"/>
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" s="8"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="7"/>
       <c r="F97" s="7"/>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" s="8"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="7"/>
       <c r="F98" s="7"/>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
@@ -1865,22 +1970,16 @@
     <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C104" s="5"/>
-      <c r="D104"/>
-      <c r="E104"/>
-      <c r="G104" s="5"/>
-    </row>
-    <row r="105" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="8"/>
-      <c r="C105" s="10"/>
-      <c r="D105" s="5"/>
-      <c r="G105" s="5"/>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F104" s="7"/>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F105" s="7"/>
     </row>
     <row r="106" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="8"/>
-      <c r="C106" s="10"/>
-      <c r="D106" s="5"/>
+      <c r="C106" s="5"/>
+      <c r="D106"/>
+      <c r="E106"/>
       <c r="G106" s="5"/>
     </row>
     <row r="107" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1897,13 +1996,13 @@
     </row>
     <row r="109" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B109" s="8"/>
-      <c r="C109" s="5"/>
+      <c r="C109" s="10"/>
       <c r="D109" s="5"/>
       <c r="G109" s="5"/>
     </row>
     <row r="110" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B110" s="8"/>
-      <c r="C110" s="5"/>
+      <c r="C110" s="10"/>
       <c r="D110" s="5"/>
       <c r="G110" s="5"/>
     </row>
@@ -1917,14 +2016,12 @@
       <c r="B112" s="8"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
       <c r="G112" s="5"/>
     </row>
     <row r="113" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B113" s="8"/>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
       <c r="G113" s="5"/>
     </row>
     <row r="114" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1962,33 +2059,33 @@
       <c r="E118" s="5"/>
       <c r="G118" s="5"/>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B119" s="8"/>
+      <c r="C119" s="5"/>
       <c r="D119" s="5"/>
       <c r="E119" s="5"/>
-      <c r="F119" s="7"/>
       <c r="G119" s="5"/>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="8"/>
+      <c r="C120" s="5"/>
       <c r="D120" s="5"/>
       <c r="E120" s="5"/>
-      <c r="F120" s="7"/>
       <c r="G120" s="5"/>
     </row>
-    <row r="121" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B121" s="8"/>
-      <c r="C121" s="5"/>
       <c r="D121" s="5"/>
       <c r="E121" s="5"/>
+      <c r="F121" s="7"/>
       <c r="G121" s="5"/>
     </row>
-    <row r="122" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B122" s="8"/>
-      <c r="C122" s="5"/>
       <c r="D122" s="5"/>
       <c r="E122" s="5"/>
-      <c r="G122" s="9"/>
+      <c r="F122" s="7"/>
+      <c r="G122" s="5"/>
     </row>
     <row r="123" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B123" s="8"/>
@@ -2002,7 +2099,7 @@
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
       <c r="E124" s="5"/>
-      <c r="G124" s="5"/>
+      <c r="G124" s="9"/>
     </row>
     <row r="125" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B125" s="8"/>
@@ -2025,11 +2122,11 @@
       <c r="E127" s="5"/>
       <c r="G127" s="5"/>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B128" s="8"/>
+      <c r="C128" s="5"/>
       <c r="D128" s="5"/>
       <c r="E128" s="5"/>
-      <c r="F128" s="7"/>
       <c r="G128" s="5"/>
     </row>
     <row r="129" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2039,24 +2136,23 @@
       <c r="E129" s="5"/>
       <c r="G129" s="5"/>
     </row>
-    <row r="130" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="8"/>
-      <c r="C130" s="5"/>
       <c r="D130" s="5"/>
       <c r="E130" s="5"/>
+      <c r="F130" s="7"/>
       <c r="G130" s="5"/>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B131" s="8"/>
-      <c r="C131" s="10"/>
+      <c r="C131" s="5"/>
       <c r="D131" s="5"/>
       <c r="E131" s="5"/>
-      <c r="F131" s="7"/>
       <c r="G131" s="5"/>
     </row>
     <row r="132" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B132" s="8"/>
-      <c r="C132" s="10"/>
+      <c r="C132" s="5"/>
       <c r="D132" s="5"/>
       <c r="E132" s="5"/>
       <c r="G132" s="5"/>
@@ -2069,60 +2165,61 @@
       <c r="F133" s="7"/>
       <c r="G133" s="5"/>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B134" s="8"/>
+      <c r="C134" s="10"/>
       <c r="D134" s="5"/>
       <c r="E134" s="5"/>
-      <c r="F134" s="7"/>
       <c r="G134" s="5"/>
     </row>
     <row r="135" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B135" s="8"/>
+      <c r="C135" s="10"/>
       <c r="D135" s="5"/>
       <c r="E135" s="5"/>
       <c r="F135" s="7"/>
       <c r="G135" s="5"/>
     </row>
-    <row r="136" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B136" s="8"/>
-      <c r="C136" s="5"/>
       <c r="D136" s="5"/>
       <c r="E136" s="5"/>
+      <c r="F136" s="7"/>
       <c r="G136" s="5"/>
     </row>
-    <row r="137" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B137" s="8"/>
-      <c r="C137" s="5"/>
       <c r="D137" s="5"/>
       <c r="E137" s="5"/>
+      <c r="F137" s="7"/>
       <c r="G137" s="5"/>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B138" s="8"/>
+      <c r="C138" s="5"/>
       <c r="D138" s="5"/>
       <c r="E138" s="5"/>
-      <c r="F138" s="7"/>
       <c r="G138" s="5"/>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B139" s="8"/>
+      <c r="C139" s="5"/>
       <c r="D139" s="5"/>
       <c r="E139" s="5"/>
-      <c r="F139" s="7"/>
       <c r="G139" s="5"/>
     </row>
-    <row r="140" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B140" s="8"/>
-      <c r="C140" s="5"/>
       <c r="D140" s="5"/>
       <c r="E140" s="5"/>
+      <c r="F140" s="7"/>
       <c r="G140" s="5"/>
     </row>
-    <row r="141" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B141" s="8"/>
-      <c r="C141" s="5"/>
       <c r="D141" s="5"/>
       <c r="E141" s="5"/>
+      <c r="F141" s="7"/>
       <c r="G141" s="5"/>
     </row>
     <row r="142" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2146,124 +2243,130 @@
       <c r="E144" s="5"/>
       <c r="G144" s="5"/>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B145" s="8"/>
+      <c r="C145" s="5"/>
       <c r="D145" s="5"/>
       <c r="E145" s="5"/>
-      <c r="F145" s="7"/>
-    </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G145" s="5"/>
+    </row>
+    <row r="146" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B146" s="8"/>
+      <c r="C146" s="5"/>
       <c r="D146" s="5"/>
       <c r="E146" s="5"/>
-      <c r="F146" s="7"/>
-    </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G146" s="5"/>
+    </row>
+    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147" s="8"/>
       <c r="D147" s="5"/>
       <c r="E147" s="5"/>
       <c r="F147" s="7"/>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B148" s="2"/>
+    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B148" s="8"/>
+      <c r="D148" s="5"/>
+      <c r="E148" s="5"/>
       <c r="F148" s="7"/>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B149" s="2"/>
+    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B149" s="8"/>
+      <c r="D149" s="5"/>
+      <c r="E149" s="5"/>
       <c r="F149" s="7"/>
     </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B150" s="2"/>
       <c r="F150" s="7"/>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B151" s="2"/>
       <c r="F151" s="7"/>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B152" s="2"/>
       <c r="F152" s="7"/>
     </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B153" s="2"/>
       <c r="F153" s="7"/>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B154" s="2"/>
       <c r="F154" s="7"/>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B155" s="2"/>
       <c r="F155" s="7"/>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B156" s="2"/>
       <c r="F156" s="7"/>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B157" s="2"/>
       <c r="F157" s="7"/>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B158" s="2"/>
       <c r="F158" s="7"/>
     </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B159" s="2"/>
       <c r="F159" s="7"/>
     </row>
-    <row r="160" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B160" s="2"/>
-      <c r="C160" s="5"/>
-      <c r="D160"/>
-      <c r="E160"/>
+      <c r="F160" s="7"/>
     </row>
     <row r="161" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B161" s="2"/>
       <c r="F161" s="7"/>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B162" s="2"/>
-      <c r="F162" s="7"/>
-    </row>
-    <row r="163" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C162" s="5"/>
+      <c r="D162"/>
+      <c r="E162"/>
+    </row>
+    <row r="163" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B163" s="2"/>
-      <c r="C163" s="5"/>
-    </row>
-    <row r="164" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F163" s="7"/>
+    </row>
+    <row r="164" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B164" s="2"/>
-      <c r="C164" s="5"/>
-      <c r="D164"/>
-      <c r="E164"/>
-    </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F164" s="7"/>
+    </row>
+    <row r="165" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B165" s="2"/>
-      <c r="F165" s="7"/>
-    </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C165" s="5"/>
+    </row>
+    <row r="166" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B166" s="2"/>
-      <c r="D166" s="7"/>
-      <c r="E166" s="7"/>
-      <c r="F166" s="7"/>
+      <c r="C166" s="5"/>
+      <c r="D166"/>
+      <c r="E166"/>
     </row>
     <row r="167" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B167" s="2"/>
-      <c r="D167" s="7"/>
-      <c r="E167" s="7"/>
       <c r="F167" s="7"/>
     </row>
     <row r="168" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B168" s="2"/>
-      <c r="D168" s="5"/>
-      <c r="E168" s="5"/>
+      <c r="D168" s="7"/>
+      <c r="E168" s="7"/>
       <c r="F168" s="7"/>
     </row>
     <row r="169" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B169" s="2"/>
+      <c r="D169" s="7"/>
+      <c r="E169" s="7"/>
       <c r="F169" s="7"/>
     </row>
     <row r="170" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B170" s="2"/>
+      <c r="D170" s="5"/>
+      <c r="E170" s="5"/>
       <c r="F170" s="7"/>
     </row>
     <row r="171" spans="2:6" x14ac:dyDescent="0.25">
@@ -2290,28 +2393,36 @@
       <c r="B176" s="2"/>
       <c r="F176" s="7"/>
     </row>
-    <row r="177" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B177" s="2"/>
-      <c r="C177" s="5"/>
-      <c r="D177"/>
-      <c r="E177"/>
+      <c r="F177" s="7"/>
     </row>
     <row r="178" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B178" s="2"/>
       <c r="F178" s="7"/>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B179" s="2"/>
-      <c r="F179" s="7"/>
+      <c r="C179" s="5"/>
+      <c r="D179"/>
+      <c r="E179"/>
     </row>
     <row r="180" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B180" s="2"/>
-      <c r="D180" s="5"/>
-      <c r="E180" s="5"/>
       <c r="F180" s="7"/>
     </row>
+    <row r="181" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B181" s="2"/>
+      <c r="F181" s="7"/>
+    </row>
+    <row r="182" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B182" s="2"/>
+      <c r="D182" s="5"/>
+      <c r="E182" s="5"/>
+      <c r="F182" s="7"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:G177">
+  <autoFilter ref="B1:G179">
     <sortState ref="B2:L87">
       <sortCondition ref="E1:E87"/>
     </sortState>
@@ -2328,7 +2439,7 @@
           <x14:formula1>
             <xm:f>Stats!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>D105:D180 D2:D96</xm:sqref>
+          <xm:sqref>D107:D182 D2:D98</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2752,8 +2863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2792,22 +2903,22 @@
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="G2" s="7" t="b">
         <v>1</v>
@@ -2815,22 +2926,22 @@
     </row>
     <row r="3" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="G3" s="7" t="b">
         <v>1</v>
@@ -2838,22 +2949,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="G4" s="7" t="b">
         <v>1</v>
@@ -2864,19 +2975,19 @@
         <v>64</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="G5" s="7" t="b">
         <v>1</v>
@@ -2884,22 +2995,22 @@
     </row>
     <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="G6" s="7" t="b">
         <v>1</v>
@@ -2907,22 +3018,22 @@
     </row>
     <row r="7" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="G7" s="7" t="b">
         <v>1</v>
@@ -2930,22 +3041,22 @@
     </row>
     <row r="8" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>121</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G8" s="7" t="b">
         <v>1</v>
@@ -2953,22 +3064,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>124</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G9" s="7" t="b">
         <v>1</v>
@@ -3025,7 +3136,7 @@
         <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H1" t="s">
         <v>27</v>
@@ -3201,15 +3312,15 @@
     </row>
     <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
-        <f>Achievements!A7</f>
-        <v>6</v>
+        <f>Achievements!A8</f>
+        <v>7</v>
       </c>
       <c r="B7" s="7" t="str">
-        <f>Achievements!C7</f>
+        <f>Achievements!C8</f>
         <v>Filling the Royal Treasury</v>
       </c>
       <c r="C7" s="7" t="str">
-        <f>Achievements!F7</f>
+        <f>Achievements!F8</f>
         <v>Collect 100 coins to get a 1up</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -3234,15 +3345,15 @@
     </row>
     <row r="8" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <f>Achievements!A8</f>
-        <v>7</v>
+        <f>Achievements!A9</f>
+        <v>8</v>
       </c>
       <c r="B8" s="7" t="str">
-        <f>Achievements!C8</f>
+        <f>Achievements!C9</f>
         <v>Secret Stash</v>
       </c>
       <c r="C8" s="7" t="str">
-        <f>Achievements!F8</f>
+        <f>Achievements!F9</f>
         <v>Find the secret mushroom in the castle</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -3267,15 +3378,15 @@
     </row>
     <row r="9" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
-        <f>Achievements!A9</f>
-        <v>8</v>
+        <f>Achievements!A10</f>
+        <v>9</v>
       </c>
       <c r="B9" s="7" t="str">
-        <f>Achievements!C9</f>
+        <f>Achievements!C10</f>
         <v>Winter Wonderland</v>
       </c>
       <c r="C9" s="7" t="str">
-        <f>Achievements!F9</f>
+        <f>Achievements!F10</f>
         <v xml:space="preserve">Beat level 1 </v>
       </c>
       <c r="D9" s="7" t="s">
@@ -3300,15 +3411,15 @@
     </row>
     <row r="10" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <f>Achievements!A10</f>
-        <v>9</v>
+        <f>Achievements!A11</f>
+        <v>10</v>
       </c>
       <c r="B10" s="7" t="str">
-        <f>Achievements!C10</f>
+        <f>Achievements!C11</f>
         <v>Hilltops</v>
       </c>
       <c r="C10" s="7" t="str">
-        <f>Achievements!F10</f>
+        <f>Achievements!F11</f>
         <v>Beat level 2</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -3333,15 +3444,15 @@
     </row>
     <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
-        <f>Achievements!A11</f>
-        <v>10</v>
+        <f>Achievements!A12</f>
+        <v>11</v>
       </c>
       <c r="B11" s="7" t="str">
-        <f>Achievements!C11</f>
+        <f>Achievements!C12</f>
         <v>Blooper's Garden</v>
       </c>
       <c r="C11" s="7" t="str">
-        <f>Achievements!F11</f>
+        <f>Achievements!F12</f>
         <v>Beat level 3</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -3366,15 +3477,15 @@
     </row>
     <row r="12" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <f>Achievements!A12</f>
-        <v>11</v>
+        <f>Achievements!A13</f>
+        <v>12</v>
       </c>
       <c r="B12" s="7" t="str">
-        <f>Achievements!C12</f>
+        <f>Achievements!C13</f>
         <v>Frozen Outpost</v>
       </c>
       <c r="C12" s="7" t="str">
-        <f>Achievements!F12</f>
+        <f>Achievements!F13</f>
         <v>Beat level 4</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -3399,15 +3510,15 @@
     </row>
     <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
-        <f>Achievements!A13</f>
-        <v>12</v>
+        <f>Achievements!A14</f>
+        <v>13</v>
       </c>
       <c r="B13" s="7" t="str">
-        <f>Achievements!C13</f>
+        <f>Achievements!C14</f>
         <v>Frozen Entrée</v>
       </c>
       <c r="C13" s="7" t="str">
-        <f>Achievements!F13</f>
+        <f>Achievements!F14</f>
         <v>Beat level 5</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -3432,15 +3543,15 @@
     </row>
     <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
-        <f>Achievements!A14</f>
-        <v>13</v>
+        <f>Achievements!A15</f>
+        <v>14</v>
       </c>
       <c r="B14" s="7" t="str">
-        <f>Achievements!C14</f>
+        <f>Achievements!C15</f>
         <v>Bowser The Grinch</v>
       </c>
       <c r="C14" s="7" t="str">
-        <f>Achievements!F14</f>
+        <f>Achievements!F15</f>
         <v>Beat bowser on the final level</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -3465,15 +3576,15 @@
     </row>
     <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
-        <f>Achievements!A15</f>
-        <v>14</v>
+        <f>Achievements!A21</f>
+        <v>20</v>
       </c>
       <c r="B15" s="7" t="str">
-        <f>Achievements!C15</f>
+        <f>Achievements!C21</f>
         <v>Little Lady Challenge I</v>
       </c>
       <c r="C15" s="7" t="str">
-        <f>Achievements!F15</f>
+        <f>Achievements!F21</f>
         <v>Beat level 1 without powering up</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -3498,15 +3609,15 @@
     </row>
     <row r="16" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
-        <f>Achievements!A16</f>
-        <v>15</v>
+        <f>Achievements!A22</f>
+        <v>21</v>
       </c>
       <c r="B16" s="7" t="str">
-        <f>Achievements!C16</f>
+        <f>Achievements!C22</f>
         <v>Little Lady Challenge II</v>
       </c>
       <c r="C16" s="7" t="str">
-        <f>Achievements!F16</f>
+        <f>Achievements!F22</f>
         <v>Beat level 2 without powering up</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -3531,15 +3642,15 @@
     </row>
     <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <f>Achievements!A17</f>
-        <v>16</v>
+        <f>Achievements!A23</f>
+        <v>22</v>
       </c>
       <c r="B17" s="7" t="str">
-        <f>Achievements!C17</f>
+        <f>Achievements!C23</f>
         <v>Little Lady Challenge III</v>
       </c>
       <c r="C17" s="7" t="str">
-        <f>Achievements!F17</f>
+        <f>Achievements!F23</f>
         <v>Beat level 3 without powering up</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -3564,15 +3675,15 @@
     </row>
     <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
-        <f>Achievements!A18</f>
-        <v>17</v>
+        <f>Achievements!A24</f>
+        <v>23</v>
       </c>
       <c r="B18" s="7" t="str">
-        <f>Achievements!C18</f>
+        <f>Achievements!C24</f>
         <v>Little Lady Challenge IV</v>
       </c>
       <c r="C18" s="7" t="str">
-        <f>Achievements!F18</f>
+        <f>Achievements!F24</f>
         <v>Beat level 4 without powering up</v>
       </c>
       <c r="D18" s="7" t="s">
@@ -3597,15 +3708,15 @@
     </row>
     <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
-        <f>Achievements!A19</f>
-        <v>18</v>
+        <f>Achievements!A25</f>
+        <v>24</v>
       </c>
       <c r="B19" s="7" t="str">
-        <f>Achievements!C19</f>
+        <f>Achievements!C25</f>
         <v>Little Lady Challenge V</v>
       </c>
       <c r="C19" s="7" t="str">
-        <f>Achievements!F19</f>
+        <f>Achievements!F25</f>
         <v>Beat level 5 without powering up</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -3630,15 +3741,15 @@
     </row>
     <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
-        <f>Achievements!A20</f>
-        <v>19</v>
+        <f>Achievements!A26</f>
+        <v>25</v>
       </c>
       <c r="B20" s="7" t="str">
-        <f>Achievements!C20</f>
+        <f>Achievements!C26</f>
         <v>Little Lady Challenge VI</v>
       </c>
       <c r="C20" s="7" t="str">
-        <f>Achievements!F20</f>
+        <f>Achievements!F26</f>
         <v>Beat level 6 without powering up</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -3663,15 +3774,15 @@
     </row>
     <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
-        <f>Achievements!A21</f>
-        <v>20</v>
+        <f>Achievements!A27</f>
+        <v>26</v>
       </c>
       <c r="B21" s="7" t="str">
-        <f>Achievements!C21</f>
+        <f>Achievements!C27</f>
         <v>Little Lady World Challenge</v>
       </c>
       <c r="C21" s="7" t="str">
-        <f>Achievements!F21</f>
+        <f>Achievements!F27</f>
         <v>Beat the game without powering up</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -3696,16 +3807,16 @@
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <f>Achievements!A22</f>
-        <v>21</v>
+        <f>Achievements!A28</f>
+        <v>27</v>
       </c>
       <c r="B22" s="7" t="str">
-        <f>Achievements!C22</f>
+        <f>Achievements!C28</f>
         <v>Express Delivery World Challenge</v>
       </c>
       <c r="C22" s="7" t="str">
-        <f>Achievements!F22</f>
-        <v>Beat the game in under 7:00 minutes</v>
+        <f>Achievements!F28</f>
+        <v>Beat the game in under 6:00 minutes</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>20</v>
@@ -3729,15 +3840,15 @@
     </row>
     <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
-        <f>Achievements!A23</f>
-        <v>22</v>
+        <f>Achievements!A29</f>
+        <v>28</v>
       </c>
       <c r="B23" s="7" t="str">
-        <f>Achievements!C23</f>
+        <f>Achievements!C29</f>
         <v>Early Present I</v>
       </c>
       <c r="C23" s="7" t="str">
-        <f>Achievements!F23</f>
+        <f>Achievements!F29</f>
         <v>Find the 1up mushroom in level 1</v>
       </c>
       <c r="D23" s="7" t="s">
@@ -3762,15 +3873,15 @@
     </row>
     <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <f>Achievements!A24</f>
-        <v>23</v>
+        <f>Achievements!A30</f>
+        <v>29</v>
       </c>
       <c r="B24" s="7" t="str">
-        <f>Achievements!C24</f>
+        <f>Achievements!C30</f>
         <v>Early Present II</v>
       </c>
       <c r="C24" s="7" t="str">
-        <f>Achievements!F24</f>
+        <f>Achievements!F30</f>
         <v>Find the first 1up mushroom at the start of level 2</v>
       </c>
       <c r="D24" s="7" t="s">
@@ -3795,15 +3906,15 @@
     </row>
     <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
-        <f>Achievements!A25</f>
-        <v>24</v>
+        <f>Achievements!A31</f>
+        <v>30</v>
       </c>
       <c r="B25" s="7" t="str">
-        <f>Achievements!C25</f>
+        <f>Achievements!C31</f>
         <v>Early Present III</v>
       </c>
       <c r="C25" s="7" t="str">
-        <f>Achievements!F25</f>
+        <f>Achievements!F31</f>
         <v>Find the second 1up mushroom in the clouds of level 2</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -3828,15 +3939,15 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <f>Achievements!A26</f>
-        <v>25</v>
+        <f>Achievements!A32</f>
+        <v>31</v>
       </c>
       <c r="B26" s="7" t="str">
-        <f>Achievements!C26</f>
+        <f>Achievements!C32</f>
         <v>Early Present IV</v>
       </c>
       <c r="C26" s="7" t="str">
-        <f>Achievements!F26</f>
+        <f>Achievements!F32</f>
         <v>Find the first 1up mushroom at the start of level 4</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -3861,15 +3972,15 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
-        <f>Achievements!A27</f>
-        <v>26</v>
+        <f>Achievements!A33</f>
+        <v>32</v>
       </c>
       <c r="B27" s="7" t="str">
-        <f>Achievements!C27</f>
+        <f>Achievements!C33</f>
         <v>Early Present V</v>
       </c>
       <c r="C27" s="7" t="str">
-        <f>Achievements!F27</f>
+        <f>Achievements!F33</f>
         <v>Find the second 1up mushroom at the top of level 4</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -3894,15 +4005,15 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <f>Achievements!A28</f>
-        <v>27</v>
+        <f>Achievements!A34</f>
+        <v>33</v>
       </c>
       <c r="B28" s="7" t="str">
-        <f>Achievements!C28</f>
+        <f>Achievements!C34</f>
         <v>Early Present VI</v>
       </c>
       <c r="C28" s="7" t="str">
-        <f>Achievements!F28</f>
+        <f>Achievements!F34</f>
         <v>Find the 1up mushroom at the start level 5 above the skyline</v>
       </c>
       <c r="D28" s="7" t="s">
@@ -3927,15 +4038,15 @@
     </row>
     <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
-        <f>Achievements!A29</f>
-        <v>28</v>
+        <f>Achievements!A35</f>
+        <v>34</v>
       </c>
       <c r="B29" s="7" t="str">
-        <f>Achievements!C29</f>
+        <f>Achievements!C35</f>
         <v>Early Present VII</v>
       </c>
       <c r="C29" s="7" t="str">
-        <f>Achievements!F29</f>
+        <f>Achievements!F35</f>
         <v>Find the 1up mushroom in level 6</v>
       </c>
       <c r="D29" s="7" t="s">
@@ -4003,7 +4114,7 @@
   <dimension ref="A1:A76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4054,175 +4165,175 @@
     <row r="8" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Filling the Royal Treasury","Collect 100 coins to get a 1up", 2, trigger)</v>
+        <v>achievement("Flameproof Princess of Mirth","Become invulnerable to fireballs while wearing the candy cane suit", 0, trigger)</v>
       </c>
     </row>
     <row r="9" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Secret Stash","Find the secret mushroom in the castle", 1, trigger)</v>
+        <v>achievement("Filling the Royal Treasury","Collect 100 coins to get a 1up", 2, trigger)</v>
       </c>
     </row>
     <row r="10" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
         <f ca="1">"achievement("&amp;CHAR(34)&amp;INDIRECT("Achievements!C"&amp;(ROW()-1))&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;INDIRECT("Achievements!F"&amp;(ROW()-1))&amp;CHAR(34)&amp;", "&amp;INDIRECT("Achievements!E"&amp;(ROW()-1))&amp;", trigger)"</f>
-        <v>achievement("Winter Wonderland","Beat level 1 ", 1, trigger)</v>
+        <v>achievement("Secret Stash","Find the secret mushroom in the castle", 1, trigger)</v>
       </c>
     </row>
     <row r="11" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Hilltops","Beat level 2", 2, trigger)</v>
+        <v>achievement("Winter Wonderland","Beat level 1 ", 1, trigger)</v>
       </c>
     </row>
     <row r="12" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Blooper's Garden","Beat level 3", 3, trigger)</v>
+        <v>achievement("Hilltops","Beat level 2", 2, trigger)</v>
       </c>
     </row>
     <row r="13" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Frozen Outpost","Beat level 4", 4, trigger)</v>
+        <v>achievement("Blooper's Garden","Beat level 3", 1, trigger)</v>
       </c>
     </row>
     <row r="14" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Frozen Entrée","Beat level 5", 5, trigger)</v>
+        <v>achievement("Frozen Outpost","Beat level 4", 3, trigger)</v>
       </c>
     </row>
     <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Bowser The Grinch","Beat bowser on the final level", 5, trigger)</v>
+        <v>achievement("Frozen Entrée","Beat level 5", 2, trigger)</v>
       </c>
     </row>
     <row r="16" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Little Lady Challenge I","Beat level 1 without powering up", 2, trigger)</v>
+        <v>achievement("Bowser The Grinch","Beat bowser on the final level", 5, trigger)</v>
       </c>
     </row>
     <row r="17" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Little Lady Challenge II","Beat level 2 without powering up", 3, trigger)</v>
+        <v>achievement("Righteous Royalty","Beat level 1 without pressing the left start as small Peach", 5, trigger)</v>
       </c>
     </row>
     <row r="18" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f ca="1">"achievement("&amp;CHAR(34)&amp;INDIRECT("Achievements!C"&amp;(ROW()-1))&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;INDIRECT("Achievements!F"&amp;(ROW()-1))&amp;CHAR(34)&amp;", "&amp;INDIRECT("Achievements!E"&amp;(ROW()-1))&amp;", trigger)"</f>
-        <v>achievement("Little Lady Challenge III","Beat level 3 without powering up", 5, trigger)</v>
+        <v>achievement("Fast Flight","Beat level 2 in 15s or less", 5, trigger)</v>
       </c>
     </row>
     <row r="19" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Little Lady Challenge IV","Beat level 4 without powering up", 5, trigger)</v>
+        <v>achievement("Frozen Calamari","Beat level 4 with blooper power", 25, trigger)</v>
       </c>
     </row>
     <row r="20" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Little Lady Challenge V","Beat level 5 without powering up", 5, trigger)</v>
+        <v>achievement("Barbeque Bowser","Beat the game with fire flower power", 10, trigger)</v>
       </c>
     </row>
     <row r="21" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Little Lady Challenge VI","Beat level 6 without powering up", 10, trigger)</v>
+        <v>achievement("Sweet Victory","Beat the game with candy cane power", 10, trigger)</v>
       </c>
     </row>
     <row r="22" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Little Lady World Challenge","Beat the game without powering up", 25, trigger)</v>
+        <v>achievement("Little Lady Challenge I","Beat level 1 without powering up", 1, trigger)</v>
       </c>
     </row>
     <row r="23" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Express Delivery World Challenge","Beat the game in under 7:00 minutes", 25, trigger)</v>
+        <v>achievement("Little Lady Challenge II","Beat level 2 without powering up", 2, trigger)</v>
       </c>
     </row>
     <row r="24" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Early Present I","Find the 1up mushroom in level 1", 1, trigger)</v>
+        <v>achievement("Little Lady Challenge III","Beat level 3 without powering up", 1, trigger)</v>
       </c>
     </row>
     <row r="25" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Early Present II","Find the first 1up mushroom at the start of level 2", 1, trigger)</v>
+        <v>achievement("Little Lady Challenge IV","Beat level 4 without powering up", 4, trigger)</v>
       </c>
     </row>
     <row r="26" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Early Present III","Find the second 1up mushroom in the clouds of level 2", 1, trigger)</v>
+        <v>achievement("Little Lady Challenge V","Beat level 5 without powering up", 3, trigger)</v>
       </c>
     </row>
     <row r="27" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Early Present IV","Find the first 1up mushroom at the start of level 4", 1, trigger)</v>
+        <v>achievement("Little Lady Challenge VI","Beat level 6 without powering up", 5, trigger)</v>
       </c>
     </row>
     <row r="28" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Early Present V","Find the second 1up mushroom at the top of level 4", 1, trigger)</v>
+        <v>achievement("Little Lady World Challenge","Beat the game without powering up", 10, trigger)</v>
       </c>
     </row>
     <row r="29" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Early Present VI","Find the 1up mushroom at the start level 5 above the skyline", 1, trigger)</v>
+        <v>achievement("Express Delivery World Challenge","Beat the game in under 6:00 minutes", 25, trigger)</v>
       </c>
     </row>
     <row r="30" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Early Present VII","Find the 1up mushroom in level 6", 1, trigger)</v>
+        <v>achievement("Early Present I","Find the 1up mushroom in level 1", 1, trigger)</v>
       </c>
     </row>
     <row r="31" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("","", , trigger)</v>
+        <v>achievement("Early Present II","Find the first 1up mushroom at the start of level 2", 1, trigger)</v>
       </c>
     </row>
     <row r="32" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("","", , trigger)</v>
+        <v>achievement("Early Present III","Find the second 1up mushroom in the clouds of level 2", 1, trigger)</v>
       </c>
     </row>
     <row r="33" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="str">
         <f t="shared" ref="A33:A67" ca="1" si="1">"achievement("&amp;CHAR(34)&amp;INDIRECT("Achievements!C"&amp;(ROW()-1))&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;INDIRECT("Achievements!H"&amp;(ROW()-1))&amp;CHAR(34)&amp;", "&amp;INDIRECT("Achievements!E"&amp;(ROW()-1))&amp;", trigger)"</f>
-        <v>achievement("","", , trigger)</v>
+        <v>achievement("Early Present IV","", 1, trigger)</v>
       </c>
     </row>
     <row r="34" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>achievement("","", , trigger)</v>
+        <v>achievement("Early Present V","", 1, trigger)</v>
       </c>
     </row>
     <row r="35" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>achievement("","", , trigger)</v>
+        <v>achievement("Early Present VI","", 1, trigger)</v>
       </c>
     </row>
     <row r="36" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>achievement("","", , trigger)</v>
+        <v>achievement("Early Present VII","", 1, trigger)</v>
       </c>
     </row>
     <row r="37" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4516,18 +4627,18 @@
       </c>
       <c r="C2">
         <f>COUNTIF(Achievements!D:D,A2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F2" s="4">
         <f>COUNTIF(Achievements!B:B,E2)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="7">
         <f>SUMIF(Achievements!B:B,E2,Achievements!E:E)</f>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J2" s="1"/>
     </row>
@@ -4540,7 +4651,7 @@
       </c>
       <c r="C3">
         <f>COUNTIF(Achievements!D:D,A3)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>37</v>
@@ -4564,18 +4675,18 @@
       </c>
       <c r="C4">
         <f>COUNTIF(Achievements!D:D,A4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F4" s="4">
         <f>COUNTIF(Achievements!B:B,E4)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G4" s="7">
         <f>SUMIF(Achievements!B:B,E4,Achievements!E:E)</f>
-        <v>87</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -4633,18 +4744,18 @@
       </c>
       <c r="C7">
         <f>COUNTIF(Achievements!D:D,A7)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="3">
         <f>SUM(F2:F6)</f>
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -4656,7 +4767,7 @@
       </c>
       <c r="C8">
         <f>COUNTIF(Achievements!D:D,A8)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -4690,7 +4801,7 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3">
         <f>SUM(C2:C10)</f>
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>